<commit_message>
Added Stripcenter and label of points
</commit_message>
<xml_diff>
--- a/data/SANTA ISABEL PARIS.xlsx
+++ b/data/SANTA ISABEL PARIS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joaquin Rivano\Documents\R\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joako\Documents\capstone_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8508" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="santa isable paris" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>Comuna</t>
   </si>
@@ -99,14 +99,20 @@
   </si>
   <si>
     <t>Nunoa</t>
+  </si>
+  <si>
+    <t>Strip Center</t>
+  </si>
+  <si>
+    <t>San Francisco 531</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -139,7 +145,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,23 +425,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.59765625" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -452,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -469,7 +475,7 @@
         <v>-70.637687</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -486,7 +492,7 @@
         <v>-70.649574000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -503,7 +509,7 @@
         <v>-70.656422000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -520,7 +526,7 @@
         <v>-70.657595000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -537,7 +543,7 @@
         <v>-70.668623999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -554,7 +560,7 @@
         <v>-70.650949999999995</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -571,7 +577,7 @@
         <v>-70.664607000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -588,7 +594,7 @@
         <v>-70.652023</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -605,7 +611,7 @@
         <v>-70.642143000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -622,7 +628,7 @@
         <v>-70.681140999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -639,7 +645,7 @@
         <v>-70.629759000000007</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -656,7 +662,7 @@
         <v>-70.650751999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -673,7 +679,7 @@
         <v>-70.647975000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -690,7 +696,7 @@
         <v>-70.652023999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -705,6 +711,23 @@
       </c>
       <c r="E16" s="1">
         <v>-70.680210000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-33.450980000000001</v>
+      </c>
+      <c r="E17" s="1">
+        <v>-70.646889999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>